<commit_message>
Se trabajo en la conexion a la base de datos y creacion del CRUD
</commit_message>
<xml_diff>
--- a/datosDB.xlsx
+++ b/datosDB.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -209,7 +210,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -268,11 +269,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -559,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Creacion de lectura y eliminacion de registros en la DB con MVC
</commit_message>
<xml_diff>
--- a/datosDB.xlsx
+++ b/datosDB.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,9 +86,6 @@
     <t>HP Envy 13-AQ1001LA, Sistema Operativo Windows 10 Home, Pantalla 13" Pulgadas, 16 GB Intel Optane</t>
   </si>
   <si>
-    <t>Procesador Intel Core I5 10210U Processor 1.6 GHz</t>
-  </si>
-  <si>
     <t>RAM 16GB DDR4</t>
   </si>
   <si>
@@ -150,9 +146,6 @@
     <t>Procesador Intel Core i3 1005G1 1.20 GHz</t>
   </si>
   <si>
-    <t>Procesador Intel® Core™ I7-1065G7 Processor 1.3 GHz</t>
-  </si>
-  <si>
     <t>https://i.postimg.cc/pTLWJbYr/Escritorio-1.jpg</t>
   </si>
   <si>
@@ -202,6 +195,12 @@
   </si>
   <si>
     <t>3.799.000</t>
+  </si>
+  <si>
+    <t>Procesador Intel Core I5 10210U 1.6 GHz</t>
+  </si>
+  <si>
+    <t>Procesador Intel® Core™ I7-1065G7  1.3 GHz</t>
   </si>
 </sst>
 </file>
@@ -620,13 +619,13 @@
         <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>15</v>
@@ -640,13 +639,13 @@
         <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>16</v>
@@ -655,7 +654,7 @@
         <v>14</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>17</v>
@@ -669,28 +668,28 @@
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -698,25 +697,25 @@
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -727,25 +726,25 @@
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -755,26 +754,26 @@
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>42</v>
+      <c r="D9" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -784,23 +783,23 @@
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>44</v>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>17</v>
@@ -814,25 +813,25 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -842,26 +841,26 @@
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="H12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -871,26 +870,26 @@
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="H13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="14" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -904,8 +903,12 @@
     <hyperlink ref="D7" r:id="rId4"/>
     <hyperlink ref="D8" r:id="rId5"/>
     <hyperlink ref="D11" r:id="rId6"/>
+    <hyperlink ref="D9" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se ajusta proyecto con diseño responsive, proyecto terminado
</commit_message>
<xml_diff>
--- a/datosDB.xlsx
+++ b/datosDB.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>idProduct</t>
   </si>
@@ -68,9 +68,6 @@
     <t>https://i.postimg.cc/5jcC62cD/Portatil-2.jpg</t>
   </si>
   <si>
-    <t>RAM 8 GB DDR4</t>
-  </si>
-  <si>
     <t>4.199.000</t>
   </si>
   <si>
@@ -86,15 +83,6 @@
     <t>HP Envy 13-AQ1001LA, Sistema Operativo Windows 10 Home, Pantalla 13" Pulgadas, 16 GB Intel Optane</t>
   </si>
   <si>
-    <t>RAM 16GB DDR4</t>
-  </si>
-  <si>
-    <t>SSD 128GB</t>
-  </si>
-  <si>
-    <t>SSD 256GB</t>
-  </si>
-  <si>
     <t>Gamer Legion 5, Sistema Operativo Windows 10 HOME, Disco Híbrido 1TB HDD + , Pantalla 15.6" Pulgadas</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
     <t>Portátil ASUS X509JA-BR356T, Sistema Operativo Windows 10 Home 64bit, Pantalla: 15.6" Pulgadas</t>
   </si>
   <si>
-    <t>RAM 4 GB DDR4</t>
-  </si>
-  <si>
     <t>https://i.postimg.cc/63tw5s1z/Portatil-4.jpg</t>
   </si>
   <si>
@@ -201,6 +186,51 @@
   </si>
   <si>
     <t>Procesador Intel® Core™ I7-1065G7  1.3 GHz</t>
+  </si>
+  <si>
+    <t>RAM 32 GB DDR4</t>
+  </si>
+  <si>
+    <t>SSD 260GB</t>
+  </si>
+  <si>
+    <t>Garantía 1 Año</t>
+  </si>
+  <si>
+    <t>Garantía 3 Meses</t>
+  </si>
+  <si>
+    <t>Garantía 6 Meses</t>
+  </si>
+  <si>
+    <t>Garantía 2 Año</t>
+  </si>
+  <si>
+    <t>RAM 16GB DDR3</t>
+  </si>
+  <si>
+    <t>SSD 500GB</t>
+  </si>
+  <si>
+    <t>RAM 4 GB DDR2</t>
+  </si>
+  <si>
+    <t>RAM 8 GB DDR3</t>
+  </si>
+  <si>
+    <t>SSD 1TB</t>
+  </si>
+  <si>
+    <t>RAM 16 GB DDR3</t>
+  </si>
+  <si>
+    <t>HHDD 2TB</t>
+  </si>
+  <si>
+    <t>HHDD 500GB</t>
+  </si>
+  <si>
+    <t>RAM 32GB DDR4</t>
   </si>
 </sst>
 </file>
@@ -560,17 +590,17 @@
   <dimension ref="B3:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="45" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -584,22 +614,22 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -613,22 +643,22 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -639,25 +669,25 @@
         <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>17</v>
+      <c r="J5" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -668,25 +698,25 @@
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>25</v>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -697,25 +727,25 @@
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>30</v>
+        <v>56</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -726,25 +756,25 @@
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>35</v>
+        <v>57</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -755,25 +785,25 @@
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>41</v>
+      <c r="J9" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -784,25 +814,25 @@
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -813,25 +843,25 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>47</v>
+        <v>56</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -842,25 +872,25 @@
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>52</v>
+        <v>57</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -871,29 +901,29 @@
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J14" s="5"/>
+      <c r="I14" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>